<commit_message>
fiv one scenario, frontend
</commit_message>
<xml_diff>
--- a/prog_lang_db.xlsx
+++ b/prog_lang_db.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szewc\Documents\Notebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szewc\PycharmProjects\Inference-System-for-Selecting-the-Optimal-Programming-Language\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Programing language</t>
   </si>
@@ -50,9 +50,6 @@
     <t>C++</t>
   </si>
   <si>
-    <t>HTML/CSS</t>
-  </si>
-  <si>
     <t>PHP</t>
   </si>
   <si>
@@ -105,6 +102,12 @@
   </si>
   <si>
     <t>Security Mechanisms</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>HTML</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,24 +450,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>0.8</v>
@@ -533,7 +536,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>0.5</v>
@@ -556,7 +559,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>0.7</v>
@@ -579,7 +582,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>0.85</v>
@@ -648,7 +651,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0.65</v>
@@ -671,7 +674,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>0.29999999999999899</v>
@@ -694,7 +697,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>0.19999999999999901</v>
@@ -717,7 +720,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>0.34999999999999898</v>
@@ -763,7 +766,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>0.249999999999999</v>
@@ -809,7 +812,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>0.05</v>
@@ -832,7 +835,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18">
         <v>0.8</v>
@@ -855,7 +858,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>0.149999999999999</v>
@@ -878,7 +881,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20">
         <v>0.75</v>
@@ -901,7 +904,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21">
         <v>0.55000000000000004</v>
@@ -920,6 +923,29 @@
       </c>
       <c r="G21">
         <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22">
+        <v>0.86</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0.65</v>
+      </c>
+      <c r="G22">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update documentation, add unit and e2e tests
</commit_message>
<xml_diff>
--- a/prog_lang_db.xlsx
+++ b/prog_lang_db.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Programing language</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Easy to program</t>
   </si>
   <si>
-    <t>Python</t>
-  </si>
-  <si>
     <t>Java</t>
   </si>
   <si>
@@ -108,6 +105,18 @@
   </si>
   <si>
     <t>HTML</t>
+  </si>
+  <si>
+    <t>JavaScript/React</t>
+  </si>
+  <si>
+    <t>JavaScript/Node</t>
+  </si>
+  <si>
+    <t>Python/Flask</t>
+  </si>
+  <si>
+    <t>Python/Django</t>
   </si>
 </sst>
 </file>
@@ -426,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,27 +459,27 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2">
-        <v>0.8</v>
+        <v>0.72000000000000008</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -482,18 +491,18 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.249999999999999</v>
+        <v>0.22499999999999912</v>
       </c>
       <c r="G2">
-        <v>0.34999999999999898</v>
+        <v>0.31499999999999911</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>0.39999999999999902</v>
+        <v>0.35999999999999915</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -505,18 +514,18 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="G3">
-        <v>0.39999999999999902</v>
+        <v>0.35999999999999915</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>0.45</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -528,18 +537,18 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.6</v>
+        <v>0.54</v>
       </c>
       <c r="G4">
-        <v>0.34999999999999898</v>
+        <v>0.31499999999999911</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -551,18 +560,18 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.75</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="G5">
-        <v>0.95</v>
+        <v>0.85499999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>0.7</v>
+        <v>0.63</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -574,18 +583,18 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="G6">
-        <v>0.8</v>
+        <v>0.72000000000000008</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7">
-        <v>0.85</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -597,18 +606,18 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.85</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="G7">
-        <v>0.6</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>0.6</v>
+        <v>0.54</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -620,18 +629,18 @@
         <v>1</v>
       </c>
       <c r="F8">
+        <v>0.81</v>
+      </c>
+      <c r="G8">
         <v>0.9</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>0.95</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -643,41 +652,41 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G9">
-        <v>0.7</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B10">
-        <v>0.65</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.39999999999999902</v>
+        <v>0.9</v>
       </c>
       <c r="G10">
-        <v>0.75</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B11">
-        <v>0.29999999999999899</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -686,21 +695,21 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>0.249999999999999</v>
+        <v>0.9</v>
       </c>
       <c r="G11">
-        <v>0.29999999999999899</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>0.19999999999999901</v>
+        <v>0.58500000000000008</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -709,21 +718,21 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.19999999999999901</v>
+        <v>0.35999999999999915</v>
       </c>
       <c r="G12">
-        <v>0.29999999999999899</v>
+        <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>0.34999999999999898</v>
+        <v>0.26999999999999907</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -735,18 +744,18 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>0.7</v>
+        <v>0.22499999999999912</v>
       </c>
       <c r="G13">
-        <v>0.45</v>
+        <v>0.26999999999999907</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.17999999999999911</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -758,38 +767,38 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>0.95</v>
+        <v>0.17999999999999911</v>
       </c>
       <c r="G14">
-        <v>0.65</v>
+        <v>0.26999999999999907</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B15">
-        <v>0.249999999999999</v>
+        <v>0.31499999999999911</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15">
-        <v>0.34999999999999898</v>
+        <v>0.63</v>
       </c>
       <c r="G15">
-        <v>0.29999999999999899</v>
+        <v>0.40500000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <v>0.9</v>
@@ -804,18 +813,18 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>0.55000000000000004</v>
+        <v>0.7</v>
       </c>
       <c r="G16">
-        <v>0.5</v>
+        <v>0.58500000000000008</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B17">
-        <v>0.05</v>
+        <v>0.85</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -824,21 +833,21 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0.29999999999999899</v>
+        <v>0.85</v>
       </c>
       <c r="G17">
-        <v>0.55000000000000004</v>
+        <v>0.58500000000000008</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B18">
-        <v>0.8</v>
+        <v>0.22499999999999912</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -847,21 +856,21 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>0.149999999999999</v>
+        <v>0.31499999999999911</v>
       </c>
       <c r="G18">
-        <v>0.29999999999999899</v>
+        <v>0.26999999999999907</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B19">
-        <v>0.149999999999999</v>
+        <v>0.81</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -873,21 +882,21 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>0.8</v>
+        <v>0.49500000000000005</v>
       </c>
       <c r="G19">
-        <v>0.29999999999999899</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>0.75</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -896,56 +905,125 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0.45</v>
+        <v>0.26999999999999907</v>
       </c>
       <c r="G20">
-        <v>0.85</v>
+        <v>0.49500000000000005</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B21">
-        <v>0.55000000000000004</v>
+        <v>0.72000000000000008</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0.65</v>
+        <v>0.13499999999999909</v>
       </c>
       <c r="G21">
-        <v>0.9</v>
+        <v>0.26999999999999907</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>0.86</v>
+        <v>0.13499999999999909</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>0.65</v>
+        <v>0.72000000000000008</v>
       </c>
       <c r="G22">
-        <v>0.5</v>
+        <v>0.26999999999999907</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="G23">
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>0.49500000000000005</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0.58500000000000008</v>
+      </c>
+      <c r="G24">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0.58500000000000008</v>
+      </c>
+      <c r="G25">
+        <v>0.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>